<commit_message>
3nm resolution for ELO cells
</commit_message>
<xml_diff>
--- a/data/cellscompared.xlsx
+++ b/data/cellscompared.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="105" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>k</t>
   </si>
@@ -37,24 +37,21 @@
     <t>V_oc_lim(V)</t>
   </si>
   <si>
-    <t>J_sc_measured (mA/cm^ 2)</t>
-  </si>
-  <si>
     <t>J_sc(mA/cm^2)</t>
   </si>
   <si>
     <t>J_0_rad(mA/cm^2)</t>
   </si>
   <si>
+    <t>J0 nr uit J0rad</t>
+  </si>
+  <si>
     <t>ERE(%)</t>
   </si>
   <si>
     <t>J0</t>
   </si>
   <si>
-    <t>J0 nr uit J0rad</t>
-  </si>
-  <si>
     <t>w1642</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>w1703</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>1.51929e-18</t>
   </si>
   <si>
@@ -242,6 +236,90 @@
   </si>
   <si>
     <t>1.91601e-18</t>
+  </si>
+  <si>
+    <t>3nm resolutie</t>
+  </si>
+  <si>
+    <t>W1689</t>
+  </si>
+  <si>
+    <t>2.61746e-18</t>
+  </si>
+  <si>
+    <t>2.06287e-16</t>
+  </si>
+  <si>
+    <t>W1683</t>
+  </si>
+  <si>
+    <t>2.58283e-18</t>
+  </si>
+  <si>
+    <t>1.05421e-16</t>
+  </si>
+  <si>
+    <t>W1670</t>
+  </si>
+  <si>
+    <t>1.72342e-18</t>
+  </si>
+  <si>
+    <t>4.49478e-17</t>
+  </si>
+  <si>
+    <t>W1664</t>
+  </si>
+  <si>
+    <t>2.89745e-18</t>
+  </si>
+  <si>
+    <t>2.09404e-16</t>
+  </si>
+  <si>
+    <t>W1662</t>
+  </si>
+  <si>
+    <t>2.92539e-18</t>
+  </si>
+  <si>
+    <t>9.52313e-17</t>
+  </si>
+  <si>
+    <t>W1660</t>
+  </si>
+  <si>
+    <t>2.65231e-18</t>
+  </si>
+  <si>
+    <t>4.20995e-16</t>
+  </si>
+  <si>
+    <t>W1657</t>
+  </si>
+  <si>
+    <t>3.16026e-18</t>
+  </si>
+  <si>
+    <t>2.91887e-16</t>
+  </si>
+  <si>
+    <t>W1642</t>
+  </si>
+  <si>
+    <t>2.52384e-18</t>
+  </si>
+  <si>
+    <t>3.70748e-16</t>
+  </si>
+  <si>
+    <t>W1632</t>
+  </si>
+  <si>
+    <t>3.04844e-18</t>
+  </si>
+  <si>
+    <t>4.48519e-16</t>
   </si>
 </sst>
 </file>
@@ -255,6 +333,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -316,9 +395,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -336,21 +418,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="E1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J1" activeCellId="0" pane="topLeft" sqref="J1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A50" activeCellId="0" pane="topLeft" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.2352941176471"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.243137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3098039215686"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -404,13 +486,10 @@
       <c r="I6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.996</v>
@@ -419,29 +498,26 @@
         <v>1.14923</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="E7" s="0" t="n">
         <v>21.2163</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">I7-E7</f>
+        <v>3.867294848018E-016</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0.266554</v>
       </c>
       <c r="I7" s="0" t="n">
-        <f aca="false">E7/(EXP(B7*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D7/(EXP(B7*$B$2/($B$1*$B$3))-1)</f>
         <v>3.877775548018E-016</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">I7-F7</f>
-        <v>3.867294848018E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -450,29 +526,26 @@
         <v>1.14567</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="E8" s="0" t="n">
         <v>19.4396</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">I8-E8</f>
+        <v>4.47056673607642E-016</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0.242615</v>
       </c>
       <c r="I8" s="0" t="n">
-        <f aca="false">E8/(EXP(B8*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D8/(EXP(B8*$B$2/($B$1*$B$3))-1)</f>
         <v>4.48159073607642E-016</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">I8-F8</f>
-        <v>4.47056673607642E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1.03</v>
@@ -481,29 +554,26 @@
         <v>1.14658</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="E9" s="0" t="n">
         <v>21.1872</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">I9-E9</f>
+        <v>1.02738041488489E-016</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1.1003</v>
       </c>
       <c r="I9" s="0" t="n">
-        <f aca="false">E9/(EXP(B9*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D9/(EXP(B9*$B$2/($B$1*$B$3))-1)</f>
         <v>1.03897741488489E-016</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <f aca="false">I9-F9</f>
-        <v>1.02738041488489E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1.01</v>
@@ -512,29 +582,26 @@
         <v>1.14609</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="E10" s="0" t="n">
         <v>21.5994</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">I10-E10</f>
+        <v>2.28452502800887E-016</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>0.517311</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">E10/(EXP(B10*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D10/(EXP(B10*$B$2/($B$1*$B$3))-1)</f>
         <v>2.29657372800887E-016</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <f aca="false">I10-F10</f>
-        <v>2.28452502800887E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1.04</v>
@@ -543,29 +610,26 @@
         <v>1.16305</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E11" s="0" t="n">
         <v>14.7383</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">I11-E11</f>
+        <v>4.86559168741767E-017</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0.856659</v>
       </c>
       <c r="I11" s="0" t="n">
-        <f aca="false">E11/(EXP(B11*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D11/(EXP(B11*$B$2/($B$1*$B$3))-1)</f>
         <v>4.90825198741767E-017</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <f aca="false">I11-F11</f>
-        <v>4.86559168741767E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1.04</v>
@@ -574,29 +638,26 @@
         <v>1.16115</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E12" s="0" t="n">
         <v>14.6284</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">I12-E12</f>
+        <v>4.82607201897442E-017</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>0.922171</v>
       </c>
       <c r="I12" s="0" t="n">
-        <f aca="false">E12/(EXP(B12*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D12/(EXP(B12*$B$2/($B$1*$B$3))-1)</f>
         <v>4.87165231897442E-017</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <f aca="false">I12-F12</f>
-        <v>4.82607201897442E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1.04</v>
@@ -605,29 +666,26 @@
         <v>1.16126</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E13" s="0" t="n">
         <v>14.3923</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">I13-E13</f>
+        <v>4.74837664181835E-017</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.918128</v>
       </c>
       <c r="I13" s="0" t="n">
-        <f aca="false">E13/(EXP(B13*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D13/(EXP(B13*$B$2/($B$1*$B$3))-1)</f>
         <v>4.79302464181835E-017</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">I13-F13</f>
-        <v>4.74837664181835E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1.01</v>
@@ -636,29 +694,26 @@
         <v>1.1611</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>15.6</v>
-      </c>
-      <c r="E14" s="0" t="n">
         <v>14.5685</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>27</v>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">I14-E14</f>
+        <v>1.54445983152992E-016</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>0.289492</v>
       </c>
       <c r="I14" s="0" t="n">
-        <f aca="false">E14/(EXP(B14*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D14/(EXP(B14*$B$2/($B$1*$B$3))-1)</f>
         <v>1.54900758152991E-016</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">I14-F14</f>
-        <v>1.54445983152992E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1.02</v>
@@ -667,29 +722,26 @@
         <v>1.16232</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E15" s="0" t="n">
         <v>14.7345</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>29</v>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">I15-E15</f>
+        <v>1.0595627875853E-016</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0.406493</v>
       </c>
       <c r="I15" s="0" t="n">
-        <f aca="false">E15/(EXP(B15*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D15/(EXP(B15*$B$2/($B$1*$B$3))-1)</f>
         <v>1.0639495275853E-016</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">I15-F15</f>
-        <v>1.0595627875853E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.03</v>
@@ -698,29 +750,26 @@
         <v>1.16218</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E16" s="0" t="n">
         <v>14.129</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>31</v>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">I16-E16</f>
+        <v>6.88627429424401E-017</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.601842</v>
       </c>
       <c r="I16" s="0" t="n">
-        <f aca="false">E16/(EXP(B16*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D16/(EXP(B16*$B$2/($B$1*$B$3))-1)</f>
         <v>6.92857569424401E-017</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">I16-F16</f>
-        <v>6.88627429424401E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -729,29 +778,26 @@
         <v>1.16043</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="E17" s="0" t="n">
         <v>13.8406</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>33</v>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">I17-E17</f>
+        <v>3.1863680249762E-016</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.137043</v>
       </c>
       <c r="I17" s="0" t="n">
-        <f aca="false">E17/(EXP(B17*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D17/(EXP(B17*$B$2/($B$1*$B$3))-1)</f>
         <v>3.1908014949762E-016</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <f aca="false">I17-F17</f>
-        <v>3.1863680249762E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1.03</v>
@@ -760,29 +806,26 @@
         <v>1.16148</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>15.8</v>
-      </c>
-      <c r="E18" s="0" t="n">
         <v>14.7114</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>35</v>
+      <c r="E18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">I18-E18</f>
+        <v>7.16891406915573E-017</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.618426</v>
       </c>
       <c r="I18" s="0" t="n">
-        <f aca="false">E18/(EXP(B18*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D18/(EXP(B18*$B$2/($B$1*$B$3))-1)</f>
         <v>7.21417286915573E-017</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <f aca="false">I18-F18</f>
-        <v>7.16891406915573E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1.02</v>
@@ -791,29 +834,26 @@
         <v>1.15948</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E19" s="0" t="n">
         <v>13.7813</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>37</v>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">I19-E19</f>
+        <v>9.90539913363958E-017</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0.453845</v>
       </c>
       <c r="I19" s="0" t="n">
-        <f aca="false">E19/(EXP(B19*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D19/(EXP(B19*$B$2/($B$1*$B$3))-1)</f>
         <v>9.95120813363958E-017</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <f aca="false">I19-F19</f>
-        <v>9.90539913363958E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1.03</v>
@@ -822,29 +862,26 @@
         <v>1.14917</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="E20" s="0" t="n">
         <v>18.3029</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">I20-E20</f>
+        <v>8.88472019377017E-017</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>0.995622</v>
       </c>
       <c r="I20" s="0" t="n">
-        <f aca="false">E20/(EXP(B20*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D20/(EXP(B20*$B$2/($B$1*$B$3))-1)</f>
         <v>8.97537179377017E-017</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <f aca="false">I20-F20</f>
-        <v>8.88472019377017E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1.01</v>
@@ -853,29 +890,26 @@
         <v>1.14101</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="0" t="n">
         <v>21.7549</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>41</v>
+      <c r="E21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">I21-E21</f>
+        <v>2.29833779166182E-016</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.629601</v>
       </c>
       <c r="I21" s="0" t="n">
-        <f aca="false">E21/(EXP(B21*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D21/(EXP(B21*$B$2/($B$1*$B$3))-1)</f>
         <v>2.31310739166181E-016</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">I21-F21</f>
-        <v>2.29833779166182E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.954</v>
@@ -884,29 +918,26 @@
         <v>1.14396</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" s="0" t="n">
         <v>22.0558</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>43</v>
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">I22-E22</f>
+        <v>2.04632815059097E-015</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.0643961</v>
       </c>
       <c r="I22" s="0" t="n">
-        <f aca="false">E22/(EXP(B22*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D22/(EXP(B22*$B$2/($B$1*$B$3))-1)</f>
         <v>2.04766440059097E-015</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <f aca="false">I22-F22</f>
-        <v>2.04632815059097E-015</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1.035</v>
@@ -914,30 +945,27 @@
       <c r="C23" s="0" t="n">
         <v>1.14751</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <v>28.7691</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>46</v>
+      <c r="E23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">I23-E23</f>
+        <v>1.14741233881266E-016</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>1.2881</v>
       </c>
       <c r="I23" s="0" t="n">
-        <f aca="false">E23/(EXP(B23*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D23/(EXP(B23*$B$2/($B$1*$B$3))-1)</f>
         <v>1.16260523881266E-016</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <f aca="false">I23-F23</f>
-        <v>1.14741233881266E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1.041</v>
@@ -946,29 +974,26 @@
         <v>1.14545</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="E24" s="0" t="n">
         <v>21.9846</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>48</v>
+      <c r="E24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">I24-E24</f>
+        <v>6.91784011365793E-017</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>1.75932</v>
       </c>
       <c r="I24" s="0" t="n">
-        <f aca="false">E24/(EXP(B24*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D24/(EXP(B24*$B$2/($B$1*$B$3))-1)</f>
         <v>7.04356811365793E-017</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <f aca="false">I24-F24</f>
-        <v>6.91784011365793E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1.036</v>
@@ -977,29 +1002,26 @@
         <v>1.14911</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>27.4</v>
-      </c>
-      <c r="E25" s="0" t="n">
         <v>29.1088</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>50</v>
+      <c r="E25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">I25-E25</f>
+        <v>1.11723482562516E-016</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>1.25845</v>
       </c>
       <c r="I25" s="0" t="n">
-        <f aca="false">E25/(EXP(B25*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D25/(EXP(B25*$B$2/($B$1*$B$3))-1)</f>
         <v>1.13168352562516E-016</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <f aca="false">I25-F25</f>
-        <v>1.11723482562516E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1.009</v>
@@ -1008,29 +1030,26 @@
         <v>1.15246</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="E26" s="0" t="n">
         <v>21.7244</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>52</v>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">I26-E26</f>
+        <v>2.39152468119466E-016</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0.389055</v>
       </c>
       <c r="I26" s="0" t="n">
-        <f aca="false">E26/(EXP(B26*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D26/(EXP(B26*$B$2/($B$1*$B$3))-1)</f>
         <v>2.40099803119466E-016</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <f aca="false">I26-F26</f>
-        <v>2.39152468119466E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.979</v>
@@ -1039,29 +1058,26 @@
         <v>1.15125</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="E27" s="0" t="n">
         <v>22.0774</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>54</v>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">I27-E27</f>
+        <v>7.78015815057052E-016</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.127743</v>
       </c>
       <c r="I27" s="0" t="n">
-        <f aca="false">E27/(EXP(B27*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D27/(EXP(B27*$B$2/($B$1*$B$3))-1)</f>
         <v>7.79024625057052E-016</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <f aca="false">I27-F27</f>
-        <v>7.78015815057052E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1.019</v>
@@ -1070,29 +1086,26 @@
         <v>1.1528</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="E28" s="0" t="n">
         <v>21.5277</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>56</v>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">I28-E28</f>
+        <v>1.60653806190978E-016</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0.565353</v>
       </c>
       <c r="I28" s="0" t="n">
-        <f aca="false">E28/(EXP(B28*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D28/(EXP(B28*$B$2/($B$1*$B$3))-1)</f>
         <v>1.61580357190978E-016</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <f aca="false">I28-F28</f>
-        <v>1.60653806190978E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1.026</v>
@@ -1101,29 +1114,26 @@
         <v>1.15149</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="E29" s="0" t="n">
         <v>29.1423</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>58</v>
+      <c r="E29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">I29-E29</f>
+        <v>1.65511884727142E-016</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.779662</v>
       </c>
       <c r="I29" s="0" t="n">
-        <f aca="false">E29/(EXP(B29*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D29/(EXP(B29*$B$2/($B$1*$B$3))-1)</f>
         <v>1.66831324727142E-016</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <f aca="false">I29-F29</f>
-        <v>1.65511884727142E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.959</v>
@@ -1132,29 +1142,26 @@
         <v>1.15206</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="E30" s="0" t="n">
         <v>20.1766</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>60</v>
+      <c r="E30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">I30-E30</f>
+        <v>1.54278708460898E-015</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>0.0571057</v>
       </c>
       <c r="I30" s="0" t="n">
-        <f aca="false">E30/(EXP(B30*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D30/(EXP(B30*$B$2/($B$1*$B$3))-1)</f>
         <v>1.54368046460898E-015</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <f aca="false">I30-F30</f>
-        <v>1.54278708460898E-015</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1.028</v>
@@ -1163,29 +1170,26 @@
         <v>1.1482</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>17.7</v>
-      </c>
-      <c r="E31" s="0" t="n">
         <v>20.5595</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>62</v>
+      <c r="E31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">I31-E31</f>
+        <v>1.07875097297655E-016</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>0.956506</v>
       </c>
       <c r="I31" s="0" t="n">
-        <f aca="false">E31/(EXP(B31*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D31/(EXP(B31*$B$2/($B$1*$B$3))-1)</f>
         <v>1.08932057297655E-016</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <f aca="false">I31-F31</f>
-        <v>1.07875097297655E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.996</v>
@@ -1194,29 +1198,26 @@
         <v>1.14386</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>19.3</v>
-      </c>
-      <c r="E32" s="0" t="n">
         <v>18.4515</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>64</v>
+      <c r="E32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">I32-E32</f>
+        <v>3.36122071760788E-016</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0.328201</v>
       </c>
       <c r="I32" s="0" t="n">
-        <f aca="false">E32/(EXP(B32*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D32/(EXP(B32*$B$2/($B$1*$B$3))-1)</f>
         <v>3.37244361760788E-016</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <f aca="false">I32-F32</f>
-        <v>3.36122071760788E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1.02</v>
@@ -1225,29 +1226,26 @@
         <v>1.14527</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="E33" s="0" t="n">
         <v>18.822</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>66</v>
+      <c r="E33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">I33-E33</f>
+        <v>1.34826143608269E-016</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0.786232</v>
       </c>
       <c r="I33" s="0" t="n">
-        <f aca="false">E33/(EXP(B33*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D33/(EXP(B33*$B$2/($B$1*$B$3))-1)</f>
         <v>1.35909993608269E-016</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <f aca="false">I33-F33</f>
-        <v>1.34826143608269E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1.052</v>
@@ -1256,29 +1254,26 @@
         <v>1.14865</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>20.6</v>
-      </c>
-      <c r="E34" s="0" t="n">
         <v>20.781</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>68</v>
+      <c r="E34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">I34-E34</f>
+        <v>4.24491934156741E-017</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>2.37897</v>
       </c>
       <c r="I34" s="0" t="n">
-        <f aca="false">E34/(EXP(B34*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D34/(EXP(B34*$B$2/($B$1*$B$3))-1)</f>
         <v>4.34992934156741E-017</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <f aca="false">I34-F34</f>
-        <v>4.24491934156741E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1.038</v>
@@ -1287,29 +1282,26 @@
         <v>1.14839</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>20.9</v>
-      </c>
-      <c r="E35" s="0" t="n">
         <v>21.051</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>70</v>
+      <c r="E35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">I35-E35</f>
+        <v>7.46722611763991E-017</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>1.39791</v>
       </c>
       <c r="I35" s="0" t="n">
-        <f aca="false">E35/(EXP(B35*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D35/(EXP(B35*$B$2/($B$1*$B$3))-1)</f>
         <v>7.57465411763991E-017</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <f aca="false">I35-F35</f>
-        <v>7.46722611763991E-017</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1.013</v>
@@ -1318,29 +1310,26 @@
         <v>1.14299</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="E36" s="0" t="n">
         <v>21.1752</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>72</v>
+      <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">I36-E36</f>
+        <v>1.99138860525639E-016</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>0.654914</v>
       </c>
       <c r="I36" s="0" t="n">
-        <f aca="false">E36/(EXP(B36*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D36/(EXP(B36*$B$2/($B$1*$B$3))-1)</f>
         <v>2.00470420525639E-016</v>
-      </c>
-      <c r="J36" s="0" t="n">
-        <f aca="false">I36-F36</f>
-        <v>1.99138860525639E-016</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1.016</v>
@@ -1349,27 +1338,250 @@
         <v>1.14154</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>26.1</v>
-      </c>
-      <c r="E37" s="0" t="n">
         <v>28.8024</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>74</v>
+      <c r="E37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">I37-E37</f>
+        <v>2.40876638859336E-016</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>0.778069</v>
       </c>
       <c r="I37" s="0" t="n">
-        <f aca="false">E37/(EXP(B37*$B$2/($B$1*$B$3))-1)</f>
+        <f aca="false">D37/(EXP(B37*$B$2/($B$1*$B$3))-1)</f>
         <v>2.42792648859336E-016</v>
       </c>
-      <c r="J37" s="0" t="n">
-        <f aca="false">I37-F37</f>
-        <v>2.40876638859336E-016</v>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="E38" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1.12322</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>19.3732</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1.25294</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1.12651</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>21.711</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>2.39142</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="A42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1.12528</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>13.8128</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>3.69267</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="A43" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1.12101</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>19.6883</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>1.36478</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1.12082</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>19.7314</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>2.98033</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+      <c r="A45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1.12116</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>18.1248</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0.626067</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="A46" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1.009</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1.12628</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>26.3237</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>1.0711</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+      <c r="A47" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1.12517</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>20.1414</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0.676141</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+      <c r="A48" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.991</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1.12021</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>20.0813</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0.675078</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A39:I39"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
@@ -1387,17 +1599,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1412,17 +1624,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>